<commit_message>
Update performance projections with new baseline measurements and TGS calculations
Major Updates:
- Update baseline: TTFT=8.336s, TPOT=53.46ms at 1600MHz
- Add Token Generation Speed (TGS) calculations for all frequencies
- Add output token rate calculations
- Update performance projections across all frequencies
- Add comprehensive TGS methodology documentation

Performance Results:
- Best TGS: 2000MHz  16.99 tokens/sec (+25% vs baseline)
- Baseline TGS: 1600MHz  13.59 tokens/sec
- Worst TGS: 600MHz  5.10 tokens/sec (-62.5% vs baseline)
- Token config: 112 input + 2 output = 114 total tokens

Files Updated:
- performance_projector.py: Enhanced with TGS calculations
- README.md: Updated with latest performance results
- TGS_CALCULATION_EXPLANATION.md: Detailed methodology guide
</commit_message>
<xml_diff>
--- a/output/llm_performance_projections.xlsx
+++ b/output/llm_performance_projections.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,6 +486,21 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
+          <t>projected_tgs</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>theoretical_tgs</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>output_token_rate</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
           <t>performance_improvement</t>
         </is>
       </c>
@@ -506,24 +521,33 @@
         <v>2.666666666626059</v>
       </c>
       <c r="E2" t="n">
-        <v>1466.666666644333</v>
+        <v>22229.33333299483</v>
       </c>
       <c r="F2" t="n">
-        <v>137.3333333312421</v>
+        <v>142.5599999978292</v>
       </c>
       <c r="G2" t="n">
-        <v>1603.999999975575</v>
+        <v>22371.89333299266</v>
       </c>
       <c r="H2" t="n">
-        <v>1466.666666666667</v>
+        <v>22229.33333333333</v>
       </c>
       <c r="I2" t="n">
-        <v>137.3333333333333</v>
+        <v>142.56</v>
       </c>
       <c r="J2" t="n">
-        <v>1604</v>
+        <v>22371.89333333333</v>
       </c>
       <c r="K2" t="n">
+        <v>5.095679578977786</v>
+      </c>
+      <c r="L2" t="n">
+        <v>5.095679578900191</v>
+      </c>
+      <c r="M2" t="n">
+        <v>14.02918069606099</v>
+      </c>
+      <c r="N2" t="n">
         <v>-62.49999999942897</v>
       </c>
     </row>
@@ -543,25 +567,34 @@
         <v>1.6</v>
       </c>
       <c r="E3" t="n">
-        <v>880</v>
+        <v>13337.6</v>
       </c>
       <c r="F3" t="n">
-        <v>82.40000000000001</v>
+        <v>85.536</v>
       </c>
       <c r="G3" t="n">
-        <v>962.4</v>
+        <v>13423.136</v>
       </c>
       <c r="H3" t="n">
-        <v>880</v>
+        <v>13337.6</v>
       </c>
       <c r="I3" t="n">
-        <v>82.40000000000001</v>
+        <v>85.536</v>
       </c>
       <c r="J3" t="n">
-        <v>962.4</v>
+        <v>13423.136</v>
       </c>
       <c r="K3" t="n">
-        <v>-37.5</v>
+        <v>8.492799298166984</v>
+      </c>
+      <c r="L3" t="n">
+        <v>8.492799298166984</v>
+      </c>
+      <c r="M3" t="n">
+        <v>23.38196782641227</v>
+      </c>
+      <c r="N3" t="n">
+        <v>-37.50000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -580,24 +613,33 @@
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>550</v>
+        <v>8336</v>
       </c>
       <c r="F4" t="n">
-        <v>51.5</v>
+        <v>53.46</v>
       </c>
       <c r="G4" t="n">
-        <v>601.5</v>
+        <v>8389.459999999999</v>
       </c>
       <c r="H4" t="n">
-        <v>550</v>
+        <v>8336</v>
       </c>
       <c r="I4" t="n">
-        <v>51.5</v>
+        <v>53.46</v>
       </c>
       <c r="J4" t="n">
-        <v>601.5</v>
+        <v>8389.459999999999</v>
       </c>
       <c r="K4" t="n">
+        <v>13.58847887706718</v>
+      </c>
+      <c r="L4" t="n">
+        <v>13.58847887706718</v>
+      </c>
+      <c r="M4" t="n">
+        <v>37.41114852225963</v>
+      </c>
+      <c r="N4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -617,25 +659,34 @@
         <v>0.8</v>
       </c>
       <c r="E5" t="n">
-        <v>440</v>
+        <v>6668.8</v>
       </c>
       <c r="F5" t="n">
-        <v>41.2</v>
+        <v>42.768</v>
       </c>
       <c r="G5" t="n">
-        <v>481.2</v>
+        <v>6711.568</v>
       </c>
       <c r="H5" t="n">
-        <v>440</v>
+        <v>6668.8</v>
       </c>
       <c r="I5" t="n">
-        <v>41.2</v>
+        <v>42.768</v>
       </c>
       <c r="J5" t="n">
-        <v>481.2</v>
+        <v>6711.568</v>
       </c>
       <c r="K5" t="n">
-        <v>25</v>
+        <v>16.98559859633397</v>
+      </c>
+      <c r="L5" t="n">
+        <v>16.98559859633397</v>
+      </c>
+      <c r="M5" t="n">
+        <v>46.76393565282454</v>
+      </c>
+      <c r="N5" t="n">
+        <v>24.99999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>